<commit_message>
Update results and some report
</commit_message>
<xml_diff>
--- a/labs/lab1/results.xlsx
+++ b/labs/lab1/results.xlsx
@@ -19,25 +19,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Epoch_28</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Epoch_14</t>
+  </si>
+  <si>
+    <t>Epoch_GPU</t>
+  </si>
+  <si>
+    <t>batch-size = 32</t>
+  </si>
+  <si>
+    <t>batch-size = 64</t>
+  </si>
+  <si>
+    <t>batch-size = 80</t>
+  </si>
+  <si>
+    <t>CPU_14</t>
+  </si>
+  <si>
+    <t>CPU_28</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>CPU with 14 threads</t>
+  </si>
+  <si>
+    <t>CPU with 28 threads</t>
+  </si>
+  <si>
+    <t>Batch size = 32</t>
+  </si>
+  <si>
+    <t>Batch size = 64</t>
+  </si>
+  <si>
+    <t>Batch size = 80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -48,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -56,12 +95,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,29 +443,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1">
-        <v>32</v>
-      </c>
-      <c r="C1">
-        <v>64</v>
-      </c>
-      <c r="D1">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
       </c>
       <c r="G1">
         <v>32</v>
@@ -375,8 +473,20 @@
       <c r="I1">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>32</v>
+      </c>
+      <c r="N1">
+        <v>64</v>
+      </c>
+      <c r="P1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -401,8 +511,29 @@
       <c r="I2">
         <v>0.42630000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0.41920000000000002</v>
+      </c>
+      <c r="M2">
+        <v>539.29999999999995</v>
+      </c>
+      <c r="N2">
+        <v>0.42320000000000002</v>
+      </c>
+      <c r="O2">
+        <v>291</v>
+      </c>
+      <c r="P2">
+        <v>0.41920000000000002</v>
+      </c>
+      <c r="Q2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -427,8 +558,29 @@
       <c r="I3">
         <v>0.42549999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0.40350000000000003</v>
+      </c>
+      <c r="M3">
+        <v>538</v>
+      </c>
+      <c r="N3">
+        <v>0.42480000000000001</v>
+      </c>
+      <c r="O3">
+        <v>291</v>
+      </c>
+      <c r="P3">
+        <v>0.41670000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -453,8 +605,29 @@
       <c r="I4">
         <v>0.42959999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>0.39850000000000002</v>
+      </c>
+      <c r="M4">
+        <v>538</v>
+      </c>
+      <c r="N4">
+        <v>0.43049999999999999</v>
+      </c>
+      <c r="O4">
+        <v>291</v>
+      </c>
+      <c r="P4">
+        <v>0.42670000000000002</v>
+      </c>
+      <c r="Q4">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -476,8 +649,29 @@
       <c r="I5">
         <v>0.43369999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="M5">
+        <v>539</v>
+      </c>
+      <c r="N5">
+        <v>0.43190000000000001</v>
+      </c>
+      <c r="O5">
+        <v>291</v>
+      </c>
+      <c r="P5">
+        <v>0.42509999999999998</v>
+      </c>
+      <c r="Q5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -495,6 +689,275 @@
       </c>
       <c r="I6">
         <v>0.43030000000000002</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>0.1077</v>
+      </c>
+      <c r="M6">
+        <v>538</v>
+      </c>
+      <c r="N6">
+        <v>0.43280000000000002</v>
+      </c>
+      <c r="O6">
+        <v>291</v>
+      </c>
+      <c r="P6">
+        <v>0.43230000000000002</v>
+      </c>
+      <c r="Q6">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.31073333333333336</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(C2:C6)</f>
+        <v>0.425925</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE(D2:D6)</f>
+        <v>0.42626000000000008</v>
+      </c>
+      <c r="G7">
+        <f>AVERAGE(G2:G6)</f>
+        <v>0.41105999999999998</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(H2:H6)</f>
+        <v>0.42788000000000004</v>
+      </c>
+      <c r="I7">
+        <f>AVERAGE(I2:I6)</f>
+        <v>0.42908000000000002</v>
+      </c>
+      <c r="L7">
+        <f>AVERAGE(L2:L6)</f>
+        <v>0.34758</v>
+      </c>
+      <c r="M7">
+        <v>538</v>
+      </c>
+      <c r="N7">
+        <f>AVERAGE(N2:N6)</f>
+        <v>0.42864000000000002</v>
+      </c>
+      <c r="O7">
+        <v>291</v>
+      </c>
+      <c r="P7">
+        <f>AVERAGE(P2:P6)</f>
+        <v>0.42400000000000004</v>
+      </c>
+      <c r="Q7">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.31073333333333336</v>
+      </c>
+      <c r="C8">
+        <v>0.425925</v>
+      </c>
+      <c r="D8">
+        <v>0.42626000000000008</v>
+      </c>
+      <c r="G8">
+        <v>0.41105999999999998</v>
+      </c>
+      <c r="H8">
+        <v>0.42788000000000004</v>
+      </c>
+      <c r="I8">
+        <v>0.42908000000000002</v>
+      </c>
+      <c r="L8">
+        <v>0.34758</v>
+      </c>
+      <c r="M8">
+        <v>0.42864000000000002</v>
+      </c>
+      <c r="N8">
+        <v>0.42400000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0.34758</v>
+      </c>
+      <c r="M9">
+        <v>0.42864000000000002</v>
+      </c>
+      <c r="N9">
+        <v>0.42400000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>0.41105999999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.31073333333333336</v>
+      </c>
+      <c r="D11">
+        <v>0.34758</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>0.42788000000000004</v>
+      </c>
+      <c r="C12">
+        <v>0.425925</v>
+      </c>
+      <c r="D12">
+        <v>0.42864000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>0.42908000000000002</v>
+      </c>
+      <c r="C13">
+        <v>0.42626000000000008</v>
+      </c>
+      <c r="D13">
+        <v>0.42400000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>0.40210000000000001</v>
+      </c>
+      <c r="C16">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.1077</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>0.43030000000000002</v>
+      </c>
+      <c r="C17">
+        <v>0.42949999999999999</v>
+      </c>
+      <c r="D17">
+        <v>0.43280000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>0.43030000000000002</v>
+      </c>
+      <c r="C18">
+        <v>0.43530000000000002</v>
+      </c>
+      <c r="D18">
+        <v>0.43230000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.40210000000000001</v>
+      </c>
+      <c r="C21" s="4">
+        <v>8.9800000000000005E-2</v>
+      </c>
+      <c r="D21">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.43030000000000002</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.42949999999999999</v>
+      </c>
+      <c r="D22">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.43030000000000002</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.43530000000000002</v>
+      </c>
+      <c r="D23">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update node = 2
</commit_message>
<xml_diff>
--- a/labs/lab1/results.xlsx
+++ b/labs/lab1/results.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7357A67-163F-42BD-A9CB-D0F086E48705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPU" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1349,7 +1356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1379,8 +1386,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1660,11 +1668,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="B25" sqref="B25:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,27 +2177,27 @@
         <v>1843.6</v>
       </c>
       <c r="J7">
-        <f>AVERAGE(J2:J6)</f>
+        <f t="shared" ref="J7:O7" si="1">AVERAGE(J2:J6)</f>
         <v>0.31073333333333336</v>
       </c>
       <c r="K7">
-        <f>AVERAGE(K2:K6)</f>
+        <f t="shared" si="1"/>
         <v>5235</v>
       </c>
       <c r="L7">
-        <f>AVERAGE(L2:L6)</f>
+        <f t="shared" si="1"/>
         <v>0.425925</v>
       </c>
       <c r="M7">
-        <f>AVERAGE(M2:M6)</f>
+        <f t="shared" si="1"/>
         <v>3185.2</v>
       </c>
       <c r="N7">
-        <f>AVERAGE(N2:N6)</f>
+        <f t="shared" si="1"/>
         <v>0.42626000000000008</v>
       </c>
       <c r="O7">
-        <f>AVERAGE(O2:O6)</f>
+        <f t="shared" si="1"/>
         <v>2038.6</v>
       </c>
       <c r="R7">
@@ -2507,6 +2515,60 @@
       </c>
       <c r="E23">
         <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <f>11294/B21</f>
+        <v>2.7481993381350982</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25:E25" si="2">11294/C21</f>
+        <v>2.9805763749604139</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1574021012416429</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="2"/>
+        <v>20.992565055762082</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <f t="shared" ref="B26:E26" si="3">11294/B22</f>
+        <v>3.0661888472606829</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="3"/>
+        <v>5.1840631598274127</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="3"/>
+        <v>3.545774205701369</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="3"/>
+        <v>38.81099656357388</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <f t="shared" ref="B27:E27" si="4">11294/B23</f>
+        <v>5.5243592252005476</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="4"/>
+        <v>6.1260577131698852</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="4"/>
+        <v>5.5400765231040916</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="4"/>
+        <v>41.369963369963372</v>
       </c>
     </row>
   </sheetData>
@@ -2516,7 +2578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:JY2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3822,7 +3884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>